<commit_message>
getCoursesCanRegister in courses_moderator.js is done
</commit_message>
<xml_diff>
--- a/assets/ISE Plan Info.xlsx
+++ b/assets/ISE Plan Info.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abdullah\Documents\Labs\Node js\ICS487-Project\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abdullah\Documents\Labs\Node js\ICS487-Project\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD688CDB-7F81-4372-BE2C-F801D28E17E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04A787C2-E714-44EB-B8B4-E2C702FB8B33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D939F8F1-67A8-F04D-B7BC-9A5C4BD9837F}"/>
+    <workbookView xWindow="12195" yWindow="4185" windowWidth="17250" windowHeight="8865" xr2:uid="{D939F8F1-67A8-F04D-B7BC-9A5C4BD9837F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="71">
   <si>
     <t>Course Standing</t>
   </si>
@@ -65,30 +65,18 @@
     <t>Freshman</t>
   </si>
   <si>
-    <t>Math101</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
     <t>MATH101</t>
   </si>
   <si>
-    <t>Math102</t>
-  </si>
-  <si>
     <t>Sophmore</t>
   </si>
   <si>
     <t>MATH102</t>
   </si>
   <si>
-    <t>Math201</t>
-  </si>
-  <si>
-    <t>Math208</t>
-  </si>
-  <si>
     <t>IAS121</t>
   </si>
   <si>
@@ -113,9 +101,6 @@
     <t>PHYS102</t>
   </si>
   <si>
-    <t>PHYS102-MATH102</t>
-  </si>
-  <si>
     <t>EE204</t>
   </si>
   <si>
@@ -140,9 +125,6 @@
     <t>ENG214</t>
   </si>
   <si>
-    <t>CHEM101-MATH102-PHYS102</t>
-  </si>
-  <si>
     <t>ME216-7</t>
   </si>
   <si>
@@ -161,18 +143,9 @@
     <t>ISE205</t>
   </si>
   <si>
-    <t>MATH102-ICS104</t>
-  </si>
-  <si>
-    <t>Math201-ICS104</t>
-  </si>
-  <si>
     <t>CSE301</t>
   </si>
   <si>
-    <t>Math208-EE204</t>
-  </si>
-  <si>
     <t>CISE305</t>
   </si>
   <si>
@@ -182,9 +155,6 @@
     <t>ISE303</t>
   </si>
   <si>
-    <t>JUNIOR</t>
-  </si>
-  <si>
     <t>ISE307</t>
   </si>
   <si>
@@ -200,24 +170,15 @@
     <t>ISE324</t>
   </si>
   <si>
-    <t>ISE205-ENG214-JUNIOR</t>
-  </si>
-  <si>
     <t>ISE391</t>
   </si>
   <si>
-    <t>ENG214-ISE391/499-JUNIOR</t>
-  </si>
-  <si>
     <t>ISE398</t>
   </si>
   <si>
     <t>INTERSHIP</t>
   </si>
   <si>
-    <t>ISE499-ENG214-JUNIOR</t>
-  </si>
-  <si>
     <t>ISE399</t>
   </si>
   <si>
@@ -227,9 +188,6 @@
     <t>Senior</t>
   </si>
   <si>
-    <t>ISE205-ISE303</t>
-  </si>
-  <si>
     <t>ISE402</t>
   </si>
   <si>
@@ -248,9 +206,6 @@
     <t>ISE4xx</t>
   </si>
   <si>
-    <t xml:space="preserve">ENG214 </t>
-  </si>
-  <si>
     <t>GSxxx</t>
   </si>
   <si>
@@ -258,6 +213,42 @@
   </si>
   <si>
     <t>XExxx</t>
+  </si>
+  <si>
+    <t>CHEM101 MATH102 PHYS102</t>
+  </si>
+  <si>
+    <t>MATH102 ICS104</t>
+  </si>
+  <si>
+    <t>Math201 ICS104</t>
+  </si>
+  <si>
+    <t>Math208 EE204</t>
+  </si>
+  <si>
+    <t>PHYS102 MATH102</t>
+  </si>
+  <si>
+    <t>ISE205 ISE303</t>
+  </si>
+  <si>
+    <t>juniorRequired</t>
+  </si>
+  <si>
+    <t>ISE499 ENG214</t>
+  </si>
+  <si>
+    <t>ISE205 ENG214</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>ENG214 ISE391/ISE499</t>
+  </si>
+  <si>
+    <t>MATH201</t>
   </si>
 </sst>
 </file>
@@ -313,7 +304,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -336,11 +327,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -348,6 +359,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -363,10 +376,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -666,24 +675,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6620C69-A7BE-4248-A0FB-491FDEB0F9C4}">
-  <dimension ref="A1:H50"/>
+  <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F48" sqref="F48"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.5" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
-    <col min="3" max="3" width="13.59765625" customWidth="1"/>
-    <col min="4" max="4" width="12.3984375" customWidth="1"/>
+    <col min="3" max="3" width="13.625" customWidth="1"/>
+    <col min="4" max="4" width="12.375" customWidth="1"/>
     <col min="5" max="5" width="15.5" customWidth="1"/>
-    <col min="6" max="6" width="15.09765625" customWidth="1"/>
-    <col min="9" max="9" width="10.8984375" customWidth="1"/>
+    <col min="6" max="6" width="15.125" customWidth="1"/>
+    <col min="9" max="9" width="10.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -708,16 +717,23 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I1" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="E2" s="1">
         <v>4</v>
       </c>
@@ -725,23 +741,28 @@
         <v>2.6</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="1"/>
+      <c r="D3" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="E3" s="1">
         <v>4</v>
       </c>
@@ -749,23 +770,28 @@
         <v>3</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="1"/>
+        <v>70</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="E4" s="1">
         <v>3</v>
       </c>
@@ -773,23 +799,28 @@
         <v>2.74</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="1"/>
+        <v>37</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="E5" s="1">
         <v>3</v>
       </c>
@@ -797,21 +828,28 @@
         <v>2.23</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="1"/>
+      <c r="B6" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="C6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="1"/>
+        <v>13</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="E6" s="1">
         <v>2</v>
       </c>
@@ -819,21 +857,28 @@
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="1"/>
+      <c r="B7" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="C7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="1"/>
+        <v>14</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="E7" s="1">
         <v>2</v>
       </c>
@@ -841,23 +886,28 @@
         <v>1</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="1"/>
+        <v>15</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="E8" s="1">
         <v>2</v>
       </c>
@@ -865,21 +915,28 @@
         <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="1"/>
+        <v>16</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="C9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="1"/>
+        <v>17</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="E9" s="1">
         <v>2</v>
       </c>
@@ -887,21 +944,28 @@
         <v>1</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="1"/>
+      <c r="B10" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="C10" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="1"/>
+        <v>18</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="E10" s="1">
         <v>4</v>
       </c>
@@ -909,24 +973,27 @@
         <v>3.5</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E11" s="1">
         <v>4</v>
@@ -935,23 +1002,28 @@
         <v>3.1</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>25</v>
+        <v>63</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="1"/>
+        <v>21</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="E12" s="1">
         <v>3</v>
       </c>
@@ -959,22 +1031,27 @@
         <v>2.65</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="1"/>
+      <c r="B13" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="C13" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E13" s="1">
         <v>3</v>
@@ -983,21 +1060,28 @@
         <v>2.97</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="1"/>
+      <c r="B14" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="C14" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" s="1"/>
+        <v>23</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="E14" s="1">
         <v>1</v>
       </c>
@@ -1005,21 +1089,28 @@
         <v>1</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="1"/>
+      <c r="B15" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="C15" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D15" s="1"/>
+        <v>24</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="E15" s="1">
         <v>4</v>
       </c>
@@ -1027,21 +1118,28 @@
         <v>3.02</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="1"/>
+      <c r="B16" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="C16" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D16" s="1"/>
+        <v>25</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="E16" s="1">
         <v>2</v>
       </c>
@@ -1049,21 +1147,28 @@
         <v>2.84</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+      <c r="I16" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="1"/>
+      <c r="B17" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="C17" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D17" s="1"/>
+        <v>26</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="E17" s="1">
         <v>3</v>
       </c>
@@ -1071,23 +1176,28 @@
         <v>2.4300000000000002</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D18" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="E18" s="1">
         <v>3</v>
       </c>
@@ -1095,23 +1205,28 @@
         <v>2.8</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="I18" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D19" s="1"/>
+        <v>28</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="E19" s="1">
         <v>3</v>
       </c>
@@ -1119,23 +1234,28 @@
         <v>2.74</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="I19" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D20" s="1"/>
+        <v>29</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="E20" s="1">
         <v>4</v>
       </c>
@@ -1143,23 +1263,28 @@
         <v>2.4500000000000002</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+      <c r="I20" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D21" s="1"/>
+        <v>30</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="E21" s="1">
         <v>4</v>
       </c>
@@ -1167,23 +1292,28 @@
         <v>2.98</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+      <c r="I21" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D22" s="1"/>
+        <v>32</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="E22" s="1">
         <v>3</v>
       </c>
@@ -1191,21 +1321,28 @@
         <v>2.61</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+      <c r="I22" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B23" s="1"/>
+        <v>16</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="C23" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D23" s="1"/>
+        <v>33</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="E23" s="1">
         <v>3</v>
       </c>
@@ -1213,23 +1350,28 @@
         <v>1.5</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="I23" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D24" s="1"/>
+        <v>34</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="E24" s="1">
         <v>3</v>
       </c>
@@ -1237,45 +1379,57 @@
         <v>2.75</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="I24" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D25" s="1"/>
+        <v>31</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="E25" s="1">
         <v>3</v>
       </c>
       <c r="F25" s="1">
         <v>2.93</v>
       </c>
-      <c r="G25" s="1"/>
+      <c r="G25" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="H25" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="I25" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D26" s="1"/>
+        <v>35</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="E26" s="1">
         <v>3</v>
       </c>
@@ -1283,23 +1437,28 @@
         <v>2.31</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="I26" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D27" s="1"/>
+        <v>36</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="E27" s="1">
         <v>3</v>
       </c>
@@ -1307,23 +1466,28 @@
         <v>2.5</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="I27" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D28" s="1"/>
+        <v>38</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="E28" s="1">
         <v>3</v>
       </c>
@@ -1331,23 +1495,28 @@
         <v>2.83</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="I28" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D29" s="1"/>
+        <v>39</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="E29" s="1">
         <v>3</v>
       </c>
@@ -1355,23 +1524,28 @@
         <v>2.4500000000000002</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="I29" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B30" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D30" s="1"/>
+      <c r="D30" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="E30" s="1">
         <v>3</v>
       </c>
@@ -1379,22 +1553,27 @@
         <v>2.72</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="I30" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B31" s="1"/>
+        <v>16</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="C31" s="1" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="E31" s="1">
         <v>3</v>
@@ -1403,23 +1582,28 @@
         <v>2.87</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="I31" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D32" s="6"/>
+        <v>42</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>68</v>
+      </c>
       <c r="E32" s="6">
         <v>3</v>
       </c>
@@ -1427,23 +1611,28 @@
         <v>3.25</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="H32" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="I32" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D33" s="1"/>
+        <v>43</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>68</v>
+      </c>
       <c r="E33" s="1">
         <v>2</v>
       </c>
@@ -1451,23 +1640,28 @@
         <v>2.4300000000000002</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="I33" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D34" s="1"/>
+        <v>44</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>68</v>
+      </c>
       <c r="E34" s="1">
         <v>2</v>
       </c>
@@ -1475,71 +1669,86 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+      <c r="I34" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D35" s="1"/>
+        <v>45</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>68</v>
+      </c>
       <c r="E35" s="1">
         <v>6</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="I35" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D36" s="1"/>
+        <v>47</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>68</v>
+      </c>
       <c r="E36" s="1">
         <v>0</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="I36" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D37" s="1"/>
+        <v>50</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>68</v>
+      </c>
       <c r="E37" s="1">
         <v>3</v>
       </c>
@@ -1547,23 +1756,28 @@
         <v>2.76</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="I37" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D38" s="1"/>
+        <v>51</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>68</v>
+      </c>
       <c r="E38" s="1">
         <v>3</v>
       </c>
@@ -1571,23 +1785,28 @@
         <v>3.23</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+      <c r="I38" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D39" s="1"/>
+        <v>52</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>68</v>
+      </c>
       <c r="E39" s="1">
         <v>3</v>
       </c>
@@ -1595,23 +1814,28 @@
         <v>3.34</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="I39" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D40" s="1"/>
+        <v>54</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>68</v>
+      </c>
       <c r="E40" s="1">
         <v>3</v>
       </c>
@@ -1619,23 +1843,28 @@
         <v>3</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="I40" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D41" s="1"/>
+        <v>55</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>68</v>
+      </c>
       <c r="E41" s="1">
         <v>3</v>
       </c>
@@ -1643,23 +1872,28 @@
         <v>2.75</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="I41" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D42" s="1"/>
+        <v>55</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>68</v>
+      </c>
       <c r="E42" s="1">
         <v>3</v>
       </c>
@@ -1667,23 +1901,28 @@
         <v>2.75</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="I42" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D43" s="1"/>
+        <v>53</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>68</v>
+      </c>
       <c r="E43" s="1">
         <v>0</v>
       </c>
@@ -1691,23 +1930,28 @@
         <v>1</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="I43" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>70</v>
+        <v>28</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D44" s="1"/>
+        <v>56</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>68</v>
+      </c>
       <c r="E44" s="1">
         <v>3</v>
       </c>
@@ -1715,21 +1959,28 @@
         <v>2.25</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="I44" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B45" s="1"/>
+        <v>16</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="C45" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D45" s="1"/>
+        <v>57</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>68</v>
+      </c>
       <c r="E45" s="1">
         <v>1</v>
       </c>
@@ -1737,23 +1988,28 @@
         <v>1</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="I45" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D46" s="1"/>
+        <v>58</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>68</v>
+      </c>
       <c r="E46" s="1">
         <v>3</v>
       </c>
@@ -1761,13 +2017,16 @@
         <v>3</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="I46" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
       <c r="D49" s="5"/>
@@ -1776,7 +2035,7 @@
       <c r="G49" s="1"/>
       <c r="H49" s="1"/>
     </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
       <c r="D50" s="4"/>
@@ -1797,6 +2056,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EB78D60DA1872F40907CAFBA57C0851B" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ae6997490e6fb8881e8212db9056b2be">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5f99e7eb-3a60-4457-a1be-a46cfebc52bd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3965e8a9b8e880e99b8dea6c82962ea3" ns2:_="">
     <xsd:import namespace="5f99e7eb-3a60-4457-a1be-a46cfebc52bd"/>
@@ -1928,15 +2196,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F9594BAB-49E4-454D-AD78-27956C4C9676}">
   <ds:schemaRefs>
@@ -1954,6 +2213,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66A422F7-E543-434D-990E-95D38F39508D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E97ADE7-80DF-4C1A-AF5E-19D5ED36BAC7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1969,12 +2236,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66A422F7-E543-434D-990E-95D38F39508D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fix port number for deployment
</commit_message>
<xml_diff>
--- a/assets/ISE Plan Info.xlsx
+++ b/assets/ISE Plan Info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abdullah\Documents\Labs\Node js\ICS487-Project\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04A787C2-E714-44EB-B8B4-E2C702FB8B33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22555A55-4F0D-4582-9F4D-D3C5183F125B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12195" yWindow="4185" windowWidth="17250" windowHeight="8865" xr2:uid="{D939F8F1-67A8-F04D-B7BC-9A5C4BD9837F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D939F8F1-67A8-F04D-B7BC-9A5C4BD9837F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -359,8 +359,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -677,8 +677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6620C69-A7BE-4248-A0FB-491FDEB0F9C4}">
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I46" sqref="I46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1530,7 +1530,7 @@
         <v>9</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -1849,7 +1849,7 @@
         <v>9</v>
       </c>
       <c r="I40" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -2050,18 +2050,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2197,6 +2197,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66A422F7-E543-434D-990E-95D38F39508D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F9594BAB-49E4-454D-AD78-27956C4C9676}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="5f99e7eb-3a60-4457-a1be-a46cfebc52bd"/>
@@ -2208,14 +2216,6 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66A422F7-E543-434D-990E-95D38F39508D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>